<commit_message>
finished fingerprinting basic results
</commit_message>
<xml_diff>
--- a/Server/Notebooks/FINGERPRINT/results_fingerprinting.xlsx
+++ b/Server/Notebooks/FINGERPRINT/results_fingerprinting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\5th Year College\TESE\Desenvolvimento\Code\Application\findLocationApp\findLocation\Server\Notebooks\FINGERPRINT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90CFFDB-B5BB-4A17-86D9-87AFC7F2659A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EFC588-9330-447A-86DE-BE9FFC7CB5BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22682DBA-70EE-47D9-880F-69553294C7AC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="90">
   <si>
     <t>DATASET USED</t>
   </si>
@@ -95,24 +95,9 @@
     <t>CONCLUSIONS</t>
   </si>
   <si>
-    <t>* Performance increases with the amount of training data</t>
-  </si>
-  <si>
-    <t>* Performance seems to be beacon independent</t>
-  </si>
-  <si>
-    <t>* Performance in a different device doesn't seem to change in a noticable way</t>
-  </si>
-  <si>
-    <t>LINEAR REGRESSION</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
-    <t>KNN IS THE BEST ONE</t>
-  </si>
-  <si>
     <t>FINGERPRINTING CLASSIFICATION RESULTS</t>
   </si>
   <si>
@@ -291,6 +276,33 @@
   </si>
   <si>
     <t>2.210096</t>
+  </si>
+  <si>
+    <t>0.735767</t>
+  </si>
+  <si>
+    <t>1.028073</t>
+  </si>
+  <si>
+    <t>0.879875</t>
+  </si>
+  <si>
+    <t>1.345242</t>
+  </si>
+  <si>
+    <t>1.201112</t>
+  </si>
+  <si>
+    <t>1.406280</t>
+  </si>
+  <si>
+    <t>1.579692</t>
+  </si>
+  <si>
+    <t>* Performance depends on the environment (Radio map doesn't generalize to different environments)</t>
+  </si>
+  <si>
+    <t>Random Forest and KNN seem to work if the zone is radio mapped</t>
   </si>
 </sst>
 </file>
@@ -570,20 +582,20 @@
     <xf numFmtId="49" fontId="4" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="202">
+  <dxfs count="142">
     <dxf>
       <fill>
         <patternFill>
@@ -608,6 +620,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -623,6 +649,48 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -698,41 +766,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -781,6 +814,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -796,6 +843,48 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -871,41 +960,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -933,7 +987,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -961,14 +1022,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1106,7 +1160,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1134,14 +1195,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1217,83 +1271,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -1315,263 +1292,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1600,7 +1320,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1614,158 +1334,6 @@
           <color auto="1"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1864,6 +1432,388 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
@@ -1944,15 +1894,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1965,6 +1914,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1984,15 +1935,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -2005,6 +1955,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2024,46 +1976,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2087,350 +1999,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4089,6 +3657,9 @@
                 <c:pt idx="2">
                   <c:v>0.94114500000000001</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73576699999999995</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4478,6 +4049,9 @@
                 <c:pt idx="2">
                   <c:v>-4.3778280000000001</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.36699100000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4699,7 +4273,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> / BIG DATASET</a:t>
+              <a:t> / BLE v2</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4845,10 +4419,10 @@
                   <c:v>KNN</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>LINEAR REGRESSION</c:v>
+                  <c:v>SVM</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>SVM</c:v>
+                  <c:v>RF</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>MLP</c:v>
@@ -4863,16 +4437,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.456959</c:v>
+                  <c:v>-2.5404529999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54992600000000003</c:v>
+                  <c:v>-0.987927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73137399999999997</c:v>
+                  <c:v>-2.577391</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57833100000000004</c:v>
+                  <c:v>-0.91889900000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7379,16 +6953,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>691786</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>20001</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1375951</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>101643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>200568</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>97154</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>2176</xdr:rowOff>
+      <xdr:rowOff>139880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7417,55 +6991,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80D23CFC-08CC-411A-A4F1-FD79922D10A3}" name="Tabela1" displayName="Tabela1" ref="C7:L12" totalsRowShown="0" headerRowDxfId="201" dataDxfId="200" tableBorderDxfId="199">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80D23CFC-08CC-411A-A4F1-FD79922D10A3}" name="Tabela1" displayName="Tabela1" ref="C7:L12" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140" tableBorderDxfId="139">
   <autoFilter ref="C7:L12" xr:uid="{DFBD5CF0-3B05-4F18-934A-4746EEAE7074}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{26DA34DF-8177-4442-A2D3-8EB9AD72DF1F}" name="DATASET USED" dataDxfId="198"/>
-    <tableColumn id="2" xr3:uid="{0F67067D-DC1E-40F7-B158-8349CDC4D2BD}" name="NUMBER OF SAMPLES" dataDxfId="197"/>
-    <tableColumn id="3" xr3:uid="{39DF035D-1EAA-4B9F-87E6-B5266981D298}" name="TRAINING SET PERFORMANCE" dataDxfId="196"/>
-    <tableColumn id="4" xr3:uid="{2D8408D4-33AD-4CD0-8FF1-B7C4D375DBB8}" name="TEST SET USED" dataDxfId="195"/>
-    <tableColumn id="5" xr3:uid="{E30FD73D-642C-4C28-A7D5-C3657D007A79}" name="DEVICE" dataDxfId="194"/>
-    <tableColumn id="6" xr3:uid="{9AEC8ABB-593B-4AC8-92B3-C100A2126814}" name="ALGORITHM" dataDxfId="193"/>
-    <tableColumn id="7" xr3:uid="{5B7F94A2-EF15-4A03-8E8B-8FEFE4A1E148}" name="MAE" dataDxfId="192"/>
-    <tableColumn id="8" xr3:uid="{89A9952A-3310-4FAA-993F-3D39EF2C91BA}" name="RMSE" dataDxfId="191"/>
-    <tableColumn id="9" xr3:uid="{6E36E7A8-564E-4DAA-956A-4D29821E808E}" name="ACCURACY" dataDxfId="190"/>
-    <tableColumn id="10" xr3:uid="{123E2326-DCC7-449A-9982-4EEB64A1F1B6}" name="F1-SCORE" dataDxfId="189"/>
+    <tableColumn id="1" xr3:uid="{26DA34DF-8177-4442-A2D3-8EB9AD72DF1F}" name="DATASET USED" dataDxfId="138"/>
+    <tableColumn id="2" xr3:uid="{0F67067D-DC1E-40F7-B158-8349CDC4D2BD}" name="NUMBER OF SAMPLES" dataDxfId="137"/>
+    <tableColumn id="3" xr3:uid="{39DF035D-1EAA-4B9F-87E6-B5266981D298}" name="TRAINING SET PERFORMANCE" dataDxfId="136"/>
+    <tableColumn id="4" xr3:uid="{2D8408D4-33AD-4CD0-8FF1-B7C4D375DBB8}" name="TEST SET USED" dataDxfId="135"/>
+    <tableColumn id="5" xr3:uid="{E30FD73D-642C-4C28-A7D5-C3657D007A79}" name="DEVICE" dataDxfId="134"/>
+    <tableColumn id="6" xr3:uid="{9AEC8ABB-593B-4AC8-92B3-C100A2126814}" name="ALGORITHM" dataDxfId="133"/>
+    <tableColumn id="7" xr3:uid="{5B7F94A2-EF15-4A03-8E8B-8FEFE4A1E148}" name="MAE" dataDxfId="132"/>
+    <tableColumn id="8" xr3:uid="{89A9952A-3310-4FAA-993F-3D39EF2C91BA}" name="RMSE" dataDxfId="131"/>
+    <tableColumn id="9" xr3:uid="{6E36E7A8-564E-4DAA-956A-4D29821E808E}" name="ACCURACY" dataDxfId="130"/>
+    <tableColumn id="10" xr3:uid="{123E2326-DCC7-449A-9982-4EEB64A1F1B6}" name="F1-SCORE" dataDxfId="129"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F47BA2B2-6A5F-4C0F-B740-6FD24D85CCBD}" name="Tabela17" displayName="Tabela17" ref="C31:K35" totalsRowShown="0" headerRowDxfId="188" dataDxfId="187" tableBorderDxfId="186">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F47BA2B2-6A5F-4C0F-B740-6FD24D85CCBD}" name="Tabela17" displayName="Tabela17" ref="C31:K35" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127" tableBorderDxfId="126">
   <autoFilter ref="C31:K35" xr:uid="{8FD148E6-BB74-4903-B200-56E20FAD3F7B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9B699A52-34DA-48FF-8201-40A33F8DEAA9}" name="DATASET USED" dataDxfId="185"/>
-    <tableColumn id="2" xr3:uid="{38C440C5-53FA-4FC3-86C1-BBC05382945B}" name="NUMBER OF SAMPLES" dataDxfId="184"/>
-    <tableColumn id="3" xr3:uid="{2A8E7AF8-104A-44BA-AC33-41B0C6D7F8EA}" name="TRAINING SET PERFORMANCE" dataDxfId="183"/>
-    <tableColumn id="4" xr3:uid="{2C1E7EB2-341E-4D63-B851-C70DFB8523DA}" name="TEST SET USED" dataDxfId="182"/>
-    <tableColumn id="5" xr3:uid="{41AC5D33-CAF7-4135-9579-DF1EDCF9C451}" name="DEVICE" dataDxfId="181"/>
-    <tableColumn id="6" xr3:uid="{43912D0B-D8CB-49C5-89CC-FE061E8F9176}" name="ALGORITHM" dataDxfId="180"/>
-    <tableColumn id="7" xr3:uid="{1E26028C-066C-4B1A-ADB9-91AD8E90A49D}" name="MAE" dataDxfId="179"/>
-    <tableColumn id="8" xr3:uid="{2CDC372A-0CCD-48AE-8C10-2A958573A256}" name="RMSE" dataDxfId="178"/>
-    <tableColumn id="9" xr3:uid="{1FDE3A5E-AEA9-4BA4-AE30-89B596397128}" name="R2" dataDxfId="177"/>
+    <tableColumn id="1" xr3:uid="{9B699A52-34DA-48FF-8201-40A33F8DEAA9}" name="DATASET USED" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{38C440C5-53FA-4FC3-86C1-BBC05382945B}" name="NUMBER OF SAMPLES" dataDxfId="124"/>
+    <tableColumn id="3" xr3:uid="{2A8E7AF8-104A-44BA-AC33-41B0C6D7F8EA}" name="TRAINING SET PERFORMANCE" dataDxfId="123"/>
+    <tableColumn id="4" xr3:uid="{2C1E7EB2-341E-4D63-B851-C70DFB8523DA}" name="TEST SET USED" dataDxfId="122"/>
+    <tableColumn id="5" xr3:uid="{41AC5D33-CAF7-4135-9579-DF1EDCF9C451}" name="DEVICE" dataDxfId="121"/>
+    <tableColumn id="6" xr3:uid="{43912D0B-D8CB-49C5-89CC-FE061E8F9176}" name="ALGORITHM" dataDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{1E26028C-066C-4B1A-ADB9-91AD8E90A49D}" name="MAE" dataDxfId="119"/>
+    <tableColumn id="8" xr3:uid="{2CDC372A-0CCD-48AE-8C10-2A958573A256}" name="RMSE" dataDxfId="118"/>
+    <tableColumn id="9" xr3:uid="{1FDE3A5E-AEA9-4BA4-AE30-89B596397128}" name="R2" dataDxfId="117"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A6F50936-2737-43F6-B505-1A1CB374A1D6}" name="Tabela28" displayName="Tabela28" ref="C43:K47" totalsRowShown="0" headerRowDxfId="176" dataDxfId="175" tableBorderDxfId="174">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A6F50936-2737-43F6-B505-1A1CB374A1D6}" name="Tabela28" displayName="Tabela28" ref="C43:K47" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115" tableBorderDxfId="114">
   <autoFilter ref="C43:K47" xr:uid="{47CECD53-9900-4EA8-BF2F-5D0E26457539}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{47C7938A-457D-47B2-8E97-A18A74BD5FD2}" name="DATASET USED" dataDxfId="167"/>
-    <tableColumn id="2" xr3:uid="{7CA88261-8444-430C-A8E8-46E5CBDAC96F}" name="NUMBER OF SAMPLES" dataDxfId="166"/>
-    <tableColumn id="3" xr3:uid="{675E8FF8-7883-47DF-B629-5851FC05AFB6}" name="TRAINING SET PERFORMANCE" dataDxfId="165"/>
-    <tableColumn id="4" xr3:uid="{B53A96C4-1D12-4ABC-8DD4-0C92E4ACA4D8}" name="TEST SET USED" dataDxfId="173"/>
-    <tableColumn id="5" xr3:uid="{EC0DA554-107E-442D-A100-80FBBA24ED8D}" name="DEVICE" dataDxfId="172"/>
-    <tableColumn id="6" xr3:uid="{B2533DD9-5E06-4FF5-86BF-E8D7771D354D}" name="ALGORITHM" dataDxfId="160"/>
-    <tableColumn id="7" xr3:uid="{E020E96A-4865-4567-9BAC-8C1AE263B1CF}" name="MAE" dataDxfId="159"/>
-    <tableColumn id="8" xr3:uid="{16341F1A-F688-4436-9319-BA524F079D33}" name="RMSE" dataDxfId="158"/>
-    <tableColumn id="9" xr3:uid="{088318A1-1E7C-4E56-A3F0-0A062096151E}" name="R2" dataDxfId="133">
+    <tableColumn id="1" xr3:uid="{47C7938A-457D-47B2-8E97-A18A74BD5FD2}" name="DATASET USED" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{7CA88261-8444-430C-A8E8-46E5CBDAC96F}" name="NUMBER OF SAMPLES" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{675E8FF8-7883-47DF-B629-5851FC05AFB6}" name="TRAINING SET PERFORMANCE" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{B53A96C4-1D12-4ABC-8DD4-0C92E4ACA4D8}" name="TEST SET USED" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{EC0DA554-107E-442D-A100-80FBBA24ED8D}" name="DEVICE" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{B2533DD9-5E06-4FF5-86BF-E8D7771D354D}" name="ALGORITHM" dataDxfId="108"/>
+    <tableColumn id="7" xr3:uid="{E020E96A-4865-4567-9BAC-8C1AE263B1CF}" name="MAE" dataDxfId="107"/>
+    <tableColumn id="8" xr3:uid="{16341F1A-F688-4436-9319-BA524F079D33}" name="RMSE" dataDxfId="106"/>
+    <tableColumn id="9" xr3:uid="{088318A1-1E7C-4E56-A3F0-0A062096151E}" name="R2" dataDxfId="105">
       <calculatedColumnFormula array="1">-_FV( 2,"540453")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7474,18 +7048,18 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{61FFE7F8-BDFB-44D4-9347-98B8061387D4}" name="Tabela249" displayName="Tabela249" ref="C50:K54" totalsRowShown="0" headerRowDxfId="171" dataDxfId="170" tableBorderDxfId="169">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{61FFE7F8-BDFB-44D4-9347-98B8061387D4}" name="Tabela249" displayName="Tabela249" ref="C50:K54" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103" tableBorderDxfId="102">
   <autoFilter ref="C50:K54" xr:uid="{0CC6D720-2EB7-4AD3-BF62-D45B83368F42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{82DBB22A-0376-4496-8DD5-75459BAEEE30}" name="DATASET USED" dataDxfId="163"/>
-    <tableColumn id="2" xr3:uid="{41CBB1F7-215A-45A2-BA8F-32A79E3D8F61}" name="NUMBER OF SAMPLES" dataDxfId="162"/>
-    <tableColumn id="3" xr3:uid="{B587A23D-4A2D-489A-ACE6-403ED250C36C}" name="TRAINING SET PERFORMANCE" dataDxfId="161"/>
-    <tableColumn id="4" xr3:uid="{02310B5B-B568-4332-B3E5-FC21C0EAECD5}" name="TEST SET USED" dataDxfId="164"/>
-    <tableColumn id="5" xr3:uid="{1CA3382E-E907-44E3-A2E7-AA671425D9F1}" name="DEVICE" dataDxfId="168"/>
-    <tableColumn id="6" xr3:uid="{E76F86B9-986A-403D-B689-C1530CFC39FE}" name="ALGORITHM" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{3E0011D5-6EDC-4206-8F77-F47EA6CA1457}" name="MAE" dataDxfId="156"/>
-    <tableColumn id="8" xr3:uid="{8AA9FC09-AF58-4633-9A7F-DF7A77818511}" name="RMSE" dataDxfId="155"/>
-    <tableColumn id="9" xr3:uid="{BC7F5CEB-BAFA-4F93-86F6-5F886BAEEC00}" name="R2" dataDxfId="154"/>
+    <tableColumn id="1" xr3:uid="{82DBB22A-0376-4496-8DD5-75459BAEEE30}" name="DATASET USED" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{41CBB1F7-215A-45A2-BA8F-32A79E3D8F61}" name="NUMBER OF SAMPLES" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{B587A23D-4A2D-489A-ACE6-403ED250C36C}" name="TRAINING SET PERFORMANCE" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{02310B5B-B568-4332-B3E5-FC21C0EAECD5}" name="TEST SET USED" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{1CA3382E-E907-44E3-A2E7-AA671425D9F1}" name="DEVICE" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{E76F86B9-986A-403D-B689-C1530CFC39FE}" name="ALGORITHM" dataDxfId="96"/>
+    <tableColumn id="7" xr3:uid="{3E0011D5-6EDC-4206-8F77-F47EA6CA1457}" name="MAE" dataDxfId="95"/>
+    <tableColumn id="8" xr3:uid="{8AA9FC09-AF58-4633-9A7F-DF7A77818511}" name="RMSE" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{BC7F5CEB-BAFA-4F93-86F6-5F886BAEEC00}" name="R2" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7790,8 +7364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9805F76B-573A-4178-B9E3-1E65A92A3888}">
   <dimension ref="B2:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7815,54 +7389,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="B2" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
     </row>
     <row r="6" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F6" s="8" t="s">
@@ -7909,13 +7483,13 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6">
         <v>750</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>16</v>
@@ -7927,16 +7501,16 @@
         <v>11</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="O8" s="26" t="s">
         <v>11</v>
@@ -7947,13 +7521,13 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" s="6">
         <v>750</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>16</v>
@@ -7962,22 +7536,22 @@
         <v>12</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="P9" s="7">
         <v>0.96149399999999996</v>
@@ -7985,13 +7559,13 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C10" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D10" s="6">
         <v>750</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>16</v>
@@ -8003,16 +7577,16 @@
         <v>14</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="O10" s="26" t="s">
         <v>14</v>
@@ -8023,13 +7597,13 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C11" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D11" s="9">
         <v>750</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>16</v>
@@ -8038,22 +7612,22 @@
         <v>12</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="O11" s="27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P11" s="25">
         <v>0.98184800000000005</v>
@@ -8061,13 +7635,13 @@
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C12" s="9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D12" s="9">
         <v>750</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>16</v>
@@ -8079,16 +7653,16 @@
         <v>15</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="O12" s="26" t="s">
         <v>15</v>
@@ -8130,68 +7704,68 @@
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E23" s="21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
+      <c r="B26" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
     </row>
     <row r="30" spans="2:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F30" s="8" t="s">
@@ -8224,24 +7798,24 @@
         <v>17</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M31" s="14" t="s">
         <v>2</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C32" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D32" s="6">
         <v>750</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>16</v>
@@ -8253,13 +7827,13 @@
         <v>11</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M32" s="26" t="s">
         <v>11</v>
@@ -8270,13 +7844,13 @@
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C33" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D33" s="6">
         <v>750</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>16</v>
@@ -8288,13 +7862,13 @@
         <v>14</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="M33" s="26" t="s">
         <v>14</v>
@@ -8305,13 +7879,13 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C34" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D34" s="6">
         <v>750</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>16</v>
@@ -8320,19 +7894,19 @@
         <v>12</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="M34" s="26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N34" s="7">
         <v>0.94114500000000001</v>
@@ -8340,13 +7914,13 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C35" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D35" s="6">
         <v>750</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>16</v>
@@ -8357,13 +7931,21 @@
       <c r="H35" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
+      <c r="I35" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35" s="10" t="s">
+        <v>81</v>
+      </c>
       <c r="M35" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="N35" s="7"/>
+      <c r="N35" s="7">
+        <v>0.73576699999999995</v>
+      </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
@@ -8401,7 +7983,7 @@
     </row>
     <row r="42" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F42" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.3">
@@ -8430,27 +8012,27 @@
         <v>17</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M43" s="14" t="s">
         <v>2</v>
       </c>
       <c r="N43" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C44" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D44" s="6">
         <v>750</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>12</v>
@@ -8458,34 +8040,34 @@
       <c r="H44" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I44" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J44" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="K44" s="29">
+      <c r="I44" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="J44" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="K44" s="28">
         <v>-4.1769170000000004</v>
       </c>
       <c r="M44" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="N44" s="29">
+      <c r="N44" s="28">
         <v>-4.1769170000000004</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C45" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D45" s="6">
         <v>750</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>12</v>
@@ -8493,70 +8075,70 @@
       <c r="H45" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I45" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="J45" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="K45" s="29">
+      <c r="I45" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="J45" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K45" s="28">
         <v>-0.987927</v>
       </c>
       <c r="M45" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="N45" s="29">
+      <c r="N45" s="28">
         <v>-0.987927</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C46" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D46" s="6">
         <v>750</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I46" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="J46" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="K46" s="29">
+        <v>24</v>
+      </c>
+      <c r="I46" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="J46" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="28">
         <v>-4.3778280000000001</v>
       </c>
       <c r="M46" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="N46" s="29">
+        <v>24</v>
+      </c>
+      <c r="N46" s="28">
         <v>-4.3778280000000001</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D47" s="6">
         <v>750</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>12</v>
@@ -8564,20 +8146,28 @@
       <c r="H47" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
+      <c r="I47" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="J47" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="K47" s="29">
+        <v>-0.36699100000000001</v>
+      </c>
       <c r="M47" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="N47" s="29"/>
+      <c r="N47" s="28">
+        <v>-0.36699100000000001</v>
+      </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
     </row>
     <row r="49" spans="3:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F49" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="3:14" x14ac:dyDescent="0.3">
@@ -8606,27 +8196,27 @@
         <v>17</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M50" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N50" s="14" t="s">
-        <v>3</v>
+      <c r="N50" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C51" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D51" s="6">
         <v>750</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>12</v>
@@ -8634,34 +8224,34 @@
       <c r="H51" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="J51" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="K51" s="29">
+      <c r="I51" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J51" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K51" s="28">
         <v>-2.5404529999999999</v>
       </c>
-      <c r="M51" s="18" t="s">
+      <c r="M51" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="N51" s="17">
-        <v>0.456959</v>
+      <c r="N51" s="28">
+        <v>-2.5404529999999999</v>
       </c>
     </row>
     <row r="52" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C52" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D52" s="6">
         <v>750</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>12</v>
@@ -8669,69 +8259,69 @@
       <c r="H52" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I52" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="J52" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="K52" s="29">
+      <c r="I52" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="J52" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K52" s="28">
         <v>-0.987927</v>
       </c>
-      <c r="M52" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N52" s="7">
-        <v>0.54992600000000003</v>
+      <c r="M52" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N52" s="28">
+        <v>-0.987927</v>
       </c>
     </row>
     <row r="53" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C53" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D53" s="6">
         <v>750</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="I53" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="J53" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="K53" s="29">
+        <v>24</v>
+      </c>
+      <c r="I53" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="J53" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="K53" s="28">
         <v>-2.577391</v>
       </c>
-      <c r="M53" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="N53" s="7">
-        <v>0.73137399999999997</v>
+      <c r="M53" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="N53" s="28">
+        <v>-2.577391</v>
       </c>
     </row>
     <row r="54" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C54" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D54" s="6">
         <v>750</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>12</v>
@@ -8739,14 +8329,20 @@
       <c r="H54" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="30"/>
-      <c r="M54" s="11" t="s">
+      <c r="I54" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="J54" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="K54" s="29">
+        <v>-0.91889900000000002</v>
+      </c>
+      <c r="M54" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="N54" s="7">
-        <v>0.57833100000000004</v>
+      <c r="N54" s="28">
+        <v>-0.91889900000000002</v>
       </c>
     </row>
     <row r="63" spans="3:14" x14ac:dyDescent="0.3">
@@ -8756,22 +8352,12 @@
     </row>
     <row r="64" spans="3:14" x14ac:dyDescent="0.3">
       <c r="E64" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="21" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -8783,76 +8369,83 @@
     <mergeCell ref="B26:O28"/>
   </mergeCells>
   <conditionalFormatting sqref="L8:L9 L11">
-    <cfRule type="expression" dxfId="68" priority="112">
+    <cfRule type="expression" dxfId="92" priority="121">
       <formula>L8=MAX($L8:$L12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:K35">
-    <cfRule type="cellIs" dxfId="67" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="91" priority="51" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="90" priority="52" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:K46">
-    <cfRule type="cellIs" dxfId="65" priority="13" operator="greaterThan">
-      <formula>0.6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="14" operator="between">
-      <formula>0.5</formula>
-      <formula>0.599999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="15" operator="lessThan">
-      <formula>0.4999</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="37" operator="between">
-      <formula>"-10.0"</formula>
-      <formula>"0.499"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="38" operator="greaterThan">
-      <formula>"0.6"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="39" operator="between">
+    <cfRule type="cellIs" dxfId="89" priority="48" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:K53">
-    <cfRule type="cellIs" dxfId="59" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="40" operator="lessThan">
       <formula>"0.499"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="41" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="42" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="56" priority="24">
+    <cfRule type="expression" dxfId="85" priority="33">
       <formula>L12=MAX($L12:$L16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L12">
-    <cfRule type="cellIs" dxfId="55" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="32" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="cellIs" dxfId="54" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="31" operator="greaterThan">
       <formula>"0.98"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N32:N35">
-    <cfRule type="cellIs" dxfId="53" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="25" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="81" priority="26" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K34">
+    <cfRule type="cellIs" dxfId="80" priority="9" operator="greaterThan">
+      <formula>"0.91"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K44:K47">
+    <cfRule type="cellIs" dxfId="79" priority="24" operator="lessThan">
+      <formula>0.4999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="46" operator="between">
+      <formula>"-10.0"</formula>
+      <formula>"0.499"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="47" operator="greaterThan">
+      <formula>"0.6"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="23" operator="between">
+      <formula>0.5</formula>
+      <formula>0.599999</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="22" operator="greaterThan">
+      <formula>0.6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new views for tracking status
</commit_message>
<xml_diff>
--- a/Server/Notebooks/FINGERPRINT/results_fingerprinting.xlsx
+++ b/Server/Notebooks/FINGERPRINT/results_fingerprinting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\5th Year College\TESE\Desenvolvimento\Code\Application\findLocationApp\findLocation\Server\Notebooks\FINGERPRINT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A249370D-B979-4D61-8434-520B667AC0F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67EDC2C-3D3F-428A-A553-3742164BE770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22682DBA-70EE-47D9-880F-69553294C7AC}"/>
+    <workbookView minimized="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{22682DBA-70EE-47D9-880F-69553294C7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -630,38 +630,17 @@
     <xf numFmtId="2" fontId="4" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="118">
     <dxf>
       <font>
         <b/>
@@ -1931,104 +1910,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3761,6 +3642,111 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -10827,55 +10813,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80D23CFC-08CC-411A-A4F1-FD79922D10A3}" name="Tabela1" displayName="Tabela1" ref="C7:L12" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100" tableBorderDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{80D23CFC-08CC-411A-A4F1-FD79922D10A3}" name="Tabela1" displayName="Tabela1" ref="C7:L12" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="C7:L12" xr:uid="{DFBD5CF0-3B05-4F18-934A-4746EEAE7074}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{26DA34DF-8177-4442-A2D3-8EB9AD72DF1F}" name="DATASET USED" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{0F67067D-DC1E-40F7-B158-8349CDC4D2BD}" name="NUMBER OF SAMPLES" dataDxfId="97"/>
-    <tableColumn id="3" xr3:uid="{39DF035D-1EAA-4B9F-87E6-B5266981D298}" name="TRAINING SET PERFORMANCE" dataDxfId="96"/>
-    <tableColumn id="4" xr3:uid="{2D8408D4-33AD-4CD0-8FF1-B7C4D375DBB8}" name="TEST SET USED" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{E30FD73D-642C-4C28-A7D5-C3657D007A79}" name="DEVICE" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{9AEC8ABB-593B-4AC8-92B3-C100A2126814}" name="ALGORITHM" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{5B7F94A2-EF15-4A03-8E8B-8FEFE4A1E148}" name="MAE" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{89A9952A-3310-4FAA-993F-3D39EF2C91BA}" name="RMSE" dataDxfId="91"/>
-    <tableColumn id="9" xr3:uid="{6E36E7A8-564E-4DAA-956A-4D29821E808E}" name="ACCURACY" dataDxfId="90"/>
-    <tableColumn id="10" xr3:uid="{123E2326-DCC7-449A-9982-4EEB64A1F1B6}" name="F1-SCORE" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{26DA34DF-8177-4442-A2D3-8EB9AD72DF1F}" name="DATASET USED" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{0F67067D-DC1E-40F7-B158-8349CDC4D2BD}" name="NUMBER OF SAMPLES" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{39DF035D-1EAA-4B9F-87E6-B5266981D298}" name="TRAINING SET PERFORMANCE" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{2D8408D4-33AD-4CD0-8FF1-B7C4D375DBB8}" name="TEST SET USED" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{E30FD73D-642C-4C28-A7D5-C3657D007A79}" name="DEVICE" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{9AEC8ABB-593B-4AC8-92B3-C100A2126814}" name="ALGORITHM" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{5B7F94A2-EF15-4A03-8E8B-8FEFE4A1E148}" name="MAE" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{89A9952A-3310-4FAA-993F-3D39EF2C91BA}" name="RMSE" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{6E36E7A8-564E-4DAA-956A-4D29821E808E}" name="ACCURACY" dataDxfId="73"/>
+    <tableColumn id="10" xr3:uid="{123E2326-DCC7-449A-9982-4EEB64A1F1B6}" name="F1-SCORE" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F47BA2B2-6A5F-4C0F-B740-6FD24D85CCBD}" name="Tabela17" displayName="Tabela17" ref="C31:K35" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87" tableBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F47BA2B2-6A5F-4C0F-B740-6FD24D85CCBD}" name="Tabela17" displayName="Tabela17" ref="C31:K35" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" tableBorderDxfId="69">
   <autoFilter ref="C31:K35" xr:uid="{8FD148E6-BB74-4903-B200-56E20FAD3F7B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9B699A52-34DA-48FF-8201-40A33F8DEAA9}" name="DATASET USED" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{38C440C5-53FA-4FC3-86C1-BBC05382945B}" name="NUMBER OF SAMPLES" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{2A8E7AF8-104A-44BA-AC33-41B0C6D7F8EA}" name="TRAINING SET PERFORMANCE" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{2C1E7EB2-341E-4D63-B851-C70DFB8523DA}" name="TEST SET USED" dataDxfId="82"/>
-    <tableColumn id="5" xr3:uid="{41AC5D33-CAF7-4135-9579-DF1EDCF9C451}" name="DEVICE" dataDxfId="81"/>
-    <tableColumn id="6" xr3:uid="{43912D0B-D8CB-49C5-89CC-FE061E8F9176}" name="ALGORITHM" dataDxfId="80"/>
-    <tableColumn id="7" xr3:uid="{1E26028C-066C-4B1A-ADB9-91AD8E90A49D}" name="MAE" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{2CDC372A-0CCD-48AE-8C10-2A958573A256}" name="RMSE" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{1FDE3A5E-AEA9-4BA4-AE30-89B596397128}" name="R2" dataDxfId="77"/>
+    <tableColumn id="1" xr3:uid="{9B699A52-34DA-48FF-8201-40A33F8DEAA9}" name="DATASET USED" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{38C440C5-53FA-4FC3-86C1-BBC05382945B}" name="NUMBER OF SAMPLES" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{2A8E7AF8-104A-44BA-AC33-41B0C6D7F8EA}" name="TRAINING SET PERFORMANCE" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{2C1E7EB2-341E-4D63-B851-C70DFB8523DA}" name="TEST SET USED" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{41AC5D33-CAF7-4135-9579-DF1EDCF9C451}" name="DEVICE" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{43912D0B-D8CB-49C5-89CC-FE061E8F9176}" name="ALGORITHM" dataDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{1E26028C-066C-4B1A-ADB9-91AD8E90A49D}" name="MAE" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{2CDC372A-0CCD-48AE-8C10-2A958573A256}" name="RMSE" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{1FDE3A5E-AEA9-4BA4-AE30-89B596397128}" name="R2" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A6F50936-2737-43F6-B505-1A1CB374A1D6}" name="Tabela28" displayName="Tabela28" ref="C43:K47" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75" tableBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A6F50936-2737-43F6-B505-1A1CB374A1D6}" name="Tabela28" displayName="Tabela28" ref="C43:K47" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
   <autoFilter ref="C43:K47" xr:uid="{47CECD53-9900-4EA8-BF2F-5D0E26457539}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{47C7938A-457D-47B2-8E97-A18A74BD5FD2}" name="DATASET USED" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{7CA88261-8444-430C-A8E8-46E5CBDAC96F}" name="NUMBER OF SAMPLES" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{675E8FF8-7883-47DF-B629-5851FC05AFB6}" name="TRAINING SET PERFORMANCE" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{B53A96C4-1D12-4ABC-8DD4-0C92E4ACA4D8}" name="TEST SET USED" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{EC0DA554-107E-442D-A100-80FBBA24ED8D}" name="DEVICE" dataDxfId="69"/>
-    <tableColumn id="6" xr3:uid="{B2533DD9-5E06-4FF5-86BF-E8D7771D354D}" name="ALGORITHM" dataDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{E020E96A-4865-4567-9BAC-8C1AE263B1CF}" name="MAE" dataDxfId="67"/>
-    <tableColumn id="8" xr3:uid="{16341F1A-F688-4436-9319-BA524F079D33}" name="RMSE" dataDxfId="66"/>
-    <tableColumn id="9" xr3:uid="{088318A1-1E7C-4E56-A3F0-0A062096151E}" name="R2" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{47C7938A-457D-47B2-8E97-A18A74BD5FD2}" name="DATASET USED" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{7CA88261-8444-430C-A8E8-46E5CBDAC96F}" name="NUMBER OF SAMPLES" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{675E8FF8-7883-47DF-B629-5851FC05AFB6}" name="TRAINING SET PERFORMANCE" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{B53A96C4-1D12-4ABC-8DD4-0C92E4ACA4D8}" name="TEST SET USED" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{EC0DA554-107E-442D-A100-80FBBA24ED8D}" name="DEVICE" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{B2533DD9-5E06-4FF5-86BF-E8D7771D354D}" name="ALGORITHM" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{E020E96A-4865-4567-9BAC-8C1AE263B1CF}" name="MAE" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{16341F1A-F688-4436-9319-BA524F079D33}" name="RMSE" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{088318A1-1E7C-4E56-A3F0-0A062096151E}" name="R2" dataDxfId="48">
       <calculatedColumnFormula array="1">-_FV( 2,"540453")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10884,54 +10870,54 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{61FFE7F8-BDFB-44D4-9347-98B8061387D4}" name="Tabela249" displayName="Tabela249" ref="C50:K54" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{61FFE7F8-BDFB-44D4-9347-98B8061387D4}" name="Tabela249" displayName="Tabela249" ref="C50:K54" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="C50:K54" xr:uid="{0CC6D720-2EB7-4AD3-BF62-D45B83368F42}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{82DBB22A-0376-4496-8DD5-75459BAEEE30}" name="DATASET USED" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{41CBB1F7-215A-45A2-BA8F-32A79E3D8F61}" name="NUMBER OF SAMPLES" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{B587A23D-4A2D-489A-ACE6-403ED250C36C}" name="TRAINING SET PERFORMANCE" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{02310B5B-B568-4332-B3E5-FC21C0EAECD5}" name="TEST SET USED" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{1CA3382E-E907-44E3-A2E7-AA671425D9F1}" name="DEVICE" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{E76F86B9-986A-403D-B689-C1530CFC39FE}" name="ALGORITHM" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{3E0011D5-6EDC-4206-8F77-F47EA6CA1457}" name="MAE" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{8AA9FC09-AF58-4633-9A7F-DF7A77818511}" name="RMSE" dataDxfId="54"/>
-    <tableColumn id="9" xr3:uid="{BC7F5CEB-BAFA-4F93-86F6-5F886BAEEC00}" name="R2" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{82DBB22A-0376-4496-8DD5-75459BAEEE30}" name="DATASET USED" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{41CBB1F7-215A-45A2-BA8F-32A79E3D8F61}" name="NUMBER OF SAMPLES" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{B587A23D-4A2D-489A-ACE6-403ED250C36C}" name="TRAINING SET PERFORMANCE" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{02310B5B-B568-4332-B3E5-FC21C0EAECD5}" name="TEST SET USED" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{1CA3382E-E907-44E3-A2E7-AA671425D9F1}" name="DEVICE" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{E76F86B9-986A-403D-B689-C1530CFC39FE}" name="ALGORITHM" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{3E0011D5-6EDC-4206-8F77-F47EA6CA1457}" name="MAE" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{8AA9FC09-AF58-4633-9A7F-DF7A77818511}" name="RMSE" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{BC7F5CEB-BAFA-4F93-86F6-5F886BAEEC00}" name="R2" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86EB226B-9AAF-424A-8254-F445FEEE8CE0}" name="Tabela173" displayName="Tabela173" ref="C78:K82" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{86EB226B-9AAF-424A-8254-F445FEEE8CE0}" name="Tabela173" displayName="Tabela173" ref="C78:K82" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="C78:K82" xr:uid="{019A7902-81BD-4720-8A3B-4607502D0F58}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C088EB04-20B2-41DC-964C-EFA26F872006}" name="DATASET USED" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{A334EF0C-295D-45E0-81B3-DF128AAD4D50}" name="NUMBER OF SAMPLES" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{3271F5C9-28DE-4E20-B306-EB96B385BCC4}" name="TRAINING SET PERFORMANCE" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{3F4A4F48-2AA2-4B18-8340-D09DAD48664A}" name="TEST SET USED" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{601253CD-D93A-470D-97B3-3CDF871B2B39}" name="DEVICE" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{DB294BD1-63CC-4331-9982-FAA10E6ED049}" name="ALGORITHM" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{2B7FBB3A-C1FB-4331-8C2B-56F88F827318}" name="MAE" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{D45D0D9F-7A9D-4986-980C-FE44D89D0C39}" name="RMSE" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{0D31959D-E7A8-4A82-BAA9-3F9E0574AB64}" name="R2" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{C088EB04-20B2-41DC-964C-EFA26F872006}" name="DATASET USED" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{A334EF0C-295D-45E0-81B3-DF128AAD4D50}" name="NUMBER OF SAMPLES" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{3271F5C9-28DE-4E20-B306-EB96B385BCC4}" name="TRAINING SET PERFORMANCE" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{3F4A4F48-2AA2-4B18-8340-D09DAD48664A}" name="TEST SET USED" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{601253CD-D93A-470D-97B3-3CDF871B2B39}" name="DEVICE" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{DB294BD1-63CC-4331-9982-FAA10E6ED049}" name="ALGORITHM" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{2B7FBB3A-C1FB-4331-8C2B-56F88F827318}" name="MAE" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{D45D0D9F-7A9D-4986-980C-FE44D89D0C39}" name="RMSE" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{0D31959D-E7A8-4A82-BAA9-3F9E0574AB64}" name="R2" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03354D2C-C1F6-4760-B626-F9D03BAF6117}" name="Tabela284" displayName="Tabela284" ref="C90:K94" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03354D2C-C1F6-4760-B626-F9D03BAF6117}" name="Tabela284" displayName="Tabela284" ref="C90:K94" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
   <autoFilter ref="C90:K94" xr:uid="{35FB1E17-82B5-4983-A98B-5BB79048B025}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6C3E7EBD-1BAD-471C-B038-5E98F89ADEE8}" name="DATASET USED" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{A3B54D9E-A0A4-4E6D-9C60-A30E2504A255}" name="NUMBER OF SAMPLES" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{74585067-6CD7-477E-BE49-72A01EF1D6A8}" name="TRAINING SET PERFORMANCE" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{300E84A7-427F-4C76-B131-3A7CEB564284}" name="TEST SET USED" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{551A84B1-DF83-4622-AE6D-0B0A24655446}" name="DEVICE" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{5882A60D-FA4E-4D09-9CDC-5909B7FC8514}" name="ALGORITHM" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{EA309B82-E083-4FB1-995A-992EBE89F934}" name="MAE" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{ACB9CBEC-F2C1-4DD1-866E-B3067BDA8AC0}" name="RMSE" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{4A220035-6F92-4751-9F8C-E1ED49D4D881}" name="R2" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{6C3E7EBD-1BAD-471C-B038-5E98F89ADEE8}" name="DATASET USED" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{A3B54D9E-A0A4-4E6D-9C60-A30E2504A255}" name="NUMBER OF SAMPLES" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{74585067-6CD7-477E-BE49-72A01EF1D6A8}" name="TRAINING SET PERFORMANCE" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{300E84A7-427F-4C76-B131-3A7CEB564284}" name="TEST SET USED" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{551A84B1-DF83-4622-AE6D-0B0A24655446}" name="DEVICE" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{5882A60D-FA4E-4D09-9CDC-5909B7FC8514}" name="ALGORITHM" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{EA309B82-E083-4FB1-995A-992EBE89F934}" name="MAE" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{ACB9CBEC-F2C1-4DD1-866E-B3067BDA8AC0}" name="RMSE" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{4A220035-6F92-4751-9F8C-E1ED49D4D881}" name="R2" dataDxfId="12">
       <calculatedColumnFormula array="1">-_FV( 2,"540453")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -10940,18 +10926,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00F2ABAC-EDA2-40E9-96B9-9E752CE1E991}" name="Tabela2495" displayName="Tabela2495" ref="C97:K101" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00F2ABAC-EDA2-40E9-96B9-9E752CE1E991}" name="Tabela2495" displayName="Tabela2495" ref="C97:K101" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="C97:K101" xr:uid="{A29C1DFD-FE82-4164-A7D8-AA196353E6CD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3B6D27C9-7478-4FF4-8B20-90C0A6B4BD51}" name="DATASET USED" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{E156DDB2-F556-4E4D-832F-8BD5A54DC901}" name="NUMBER OF SAMPLES" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{0ED86B38-76F3-45CE-914E-F3CC586F5BF4}" name="TRAINING SET PERFORMANCE" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{04614F0D-6A07-43AA-85BF-B6B70108EFBE}" name="TEST SET USED" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{7A05CA5D-C9E9-45BB-8593-2F29673965DF}" name="DEVICE" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{88766DA0-6B66-4865-BC70-C58815CDAD6A}" name="ALGORITHM" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{86AD69B2-5023-4248-997E-97980406F9AD}" name="MAE" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{F1D939D3-5FEF-4BC2-8A1E-E12525260989}" name="RMSE" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{9B192FD9-2AF7-4BE8-ACD6-AC9E063C0146}" name="R2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3B6D27C9-7478-4FF4-8B20-90C0A6B4BD51}" name="DATASET USED" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E156DDB2-F556-4E4D-832F-8BD5A54DC901}" name="NUMBER OF SAMPLES" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0ED86B38-76F3-45CE-914E-F3CC586F5BF4}" name="TRAINING SET PERFORMANCE" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{04614F0D-6A07-43AA-85BF-B6B70108EFBE}" name="TEST SET USED" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7A05CA5D-C9E9-45BB-8593-2F29673965DF}" name="DEVICE" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{88766DA0-6B66-4865-BC70-C58815CDAD6A}" name="ALGORITHM" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{86AD69B2-5023-4248-997E-97980406F9AD}" name="MAE" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{F1D939D3-5FEF-4BC2-8A1E-E12525260989}" name="RMSE" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{9B192FD9-2AF7-4BE8-ACD6-AC9E063C0146}" name="R2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11256,7 +11242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9805F76B-573A-4178-B9E3-1E65A92A3888}">
   <dimension ref="B2:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
@@ -11281,54 +11267,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
     </row>
     <row r="6" spans="2:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F6" s="8" t="s">
@@ -11610,54 +11596,54 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
     </row>
     <row r="30" spans="2:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F30" s="8" t="s">
@@ -12253,54 +12239,54 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="30"/>
-      <c r="I73" s="30"/>
-      <c r="J73" s="30"/>
-      <c r="K73" s="30"/>
-      <c r="L73" s="30"/>
-      <c r="M73" s="30"/>
-      <c r="N73" s="30"/>
-      <c r="O73" s="30"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="31"/>
+      <c r="L73" s="31"/>
+      <c r="M73" s="31"/>
+      <c r="N73" s="31"/>
+      <c r="O73" s="31"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B74" s="30"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
-      <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="30"/>
-      <c r="J74" s="30"/>
-      <c r="K74" s="30"/>
-      <c r="L74" s="30"/>
-      <c r="M74" s="30"/>
-      <c r="N74" s="30"/>
-      <c r="O74" s="30"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="31"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31"/>
+      <c r="M74" s="31"/>
+      <c r="N74" s="31"/>
+      <c r="O74" s="31"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B75" s="30"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="30"/>
-      <c r="M75" s="30"/>
-      <c r="N75" s="30"/>
-      <c r="O75" s="30"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+      <c r="N75" s="31"/>
+      <c r="O75" s="31"/>
     </row>
     <row r="77" spans="2:15" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="F77" s="8" t="s">
@@ -12466,7 +12452,7 @@
       <c r="H82" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I82" s="31" t="s">
+      <c r="I82" s="30" t="s">
         <v>101</v>
       </c>
       <c r="J82" s="10" t="s">
@@ -12910,147 +12896,147 @@
     <mergeCell ref="B73:O75"/>
   </mergeCells>
   <conditionalFormatting sqref="L8:L9 L11">
-    <cfRule type="expression" dxfId="119" priority="138">
+    <cfRule type="expression" dxfId="117" priority="138">
       <formula>L8=MAX($L8:$L12)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:K35">
-    <cfRule type="cellIs" dxfId="118" priority="68" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="68" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="69" operator="between">
+    <cfRule type="cellIs" dxfId="115" priority="69" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:K46">
-    <cfRule type="cellIs" dxfId="116" priority="65" operator="between">
+    <cfRule type="cellIs" dxfId="114" priority="65" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:K53">
-    <cfRule type="cellIs" dxfId="115" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="57" operator="lessThan">
       <formula>"0.499"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="58" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="59" operator="between">
+    <cfRule type="cellIs" dxfId="111" priority="59" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="112" priority="50">
+    <cfRule type="expression" dxfId="110" priority="50">
       <formula>L12=MAX($L12:$L16)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L12">
-    <cfRule type="cellIs" dxfId="111" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="49" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="cellIs" dxfId="110" priority="48" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="48" operator="greaterThan">
       <formula>"0.98"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N32:N35">
-    <cfRule type="cellIs" dxfId="109" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="42" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="106" priority="43" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="107" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="26" operator="greaterThan">
       <formula>"0.91"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:K47">
-    <cfRule type="cellIs" dxfId="106" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="41" operator="lessThan">
       <formula>0.4999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="63" operator="between">
+    <cfRule type="cellIs" dxfId="103" priority="63" operator="between">
       <formula>"-10.0"</formula>
       <formula>"0.499"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="64" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="64" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="40" operator="between">
+    <cfRule type="cellIs" dxfId="101" priority="40" operator="between">
       <formula>0.5</formula>
       <formula>0.599999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="39" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="39" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K79:K82">
-    <cfRule type="cellIs" dxfId="52" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="16" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="98" priority="17" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91:K93">
-    <cfRule type="cellIs" dxfId="50" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="97" priority="15" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K98:K100">
-    <cfRule type="cellIs" dxfId="49" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="10" operator="lessThan">
       <formula>"0.499"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="11" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="94" priority="12" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K81">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="93" priority="4" operator="greaterThan">
       <formula>"0.91"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91:K94">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="5" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="91" priority="6" operator="between">
       <formula>0.5</formula>
       <formula>0.599999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="7" operator="lessThan">
       <formula>0.4999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="89" priority="13" operator="between">
       <formula>"-10.0"</formula>
       <formula>"0.499"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="88" priority="14" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N79:N82">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="greaterThan">
       <formula>"0.6"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="between">
       <formula>"0.4999"</formula>
       <formula>"0.5999"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N81">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="1" operator="greaterThan">
       <formula>"0.91"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>